<commit_message>
Problem.py and Solution.py updates
</commit_message>
<xml_diff>
--- a/Dataset/N2OR_New.xlsx
+++ b/Dataset/N2OR_New.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1B0CF7-19C3-4DD9-9CB8-57004DCD2410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07187192-71DC-471C-A47E-657393717916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -1713,7 +1713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="299">
   <si>
     <t>Metaheuristics</t>
   </si>
@@ -2908,12 +2908,6 @@
     <t>Bo Chen</t>
   </si>
   <si>
-    <t>P0, P1</t>
-  </si>
-  <si>
-    <t>P8, P9</t>
-  </si>
-  <si>
     <t>P39, P40</t>
   </si>
   <si>
@@ -2960,6 +2954,84 @@
   </si>
   <si>
     <t>Submissions_Timezones:</t>
+  </si>
+  <si>
+    <t>NEW19A21, NEW19A3756</t>
+  </si>
+  <si>
+    <t>GMT+3</t>
+  </si>
+  <si>
+    <t>GMT-6</t>
+  </si>
+  <si>
+    <t>GMT-12</t>
+  </si>
+  <si>
+    <t>GMT+6</t>
+  </si>
+  <si>
+    <t>GMT+4</t>
+  </si>
+  <si>
+    <t>GMT+8</t>
+  </si>
+  <si>
+    <t>GMT+0</t>
+  </si>
+  <si>
+    <t>GMT+1</t>
+  </si>
+  <si>
+    <t>GMT+5</t>
+  </si>
+  <si>
+    <t>GMT+7</t>
+  </si>
+  <si>
+    <t>GMT+9</t>
+  </si>
+  <si>
+    <t>GMT+10</t>
+  </si>
+  <si>
+    <t>GMT+11</t>
+  </si>
+  <si>
+    <t>GMT+12</t>
+  </si>
+  <si>
+    <t>GMT-11</t>
+  </si>
+  <si>
+    <t>GMT-10</t>
+  </si>
+  <si>
+    <t>GMT-9</t>
+  </si>
+  <si>
+    <t>GMT-8</t>
+  </si>
+  <si>
+    <t>GMT-7</t>
+  </si>
+  <si>
+    <t>GMT-5</t>
+  </si>
+  <si>
+    <t>GMT-4</t>
+  </si>
+  <si>
+    <t>GMT-3</t>
+  </si>
+  <si>
+    <t>GMT-2</t>
+  </si>
+  <si>
+    <t>GMT-1</t>
+  </si>
+  <si>
+    <t>P12, P13, P11</t>
   </si>
 </sst>
 </file>
@@ -4834,8 +4906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B4773B-09CB-4AE1-B7A2-EA1A4F4D3191}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4870,7 +4942,7 @@
         <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>99</v>
@@ -4910,7 +4982,7 @@
         <v>92</v>
       </c>
       <c r="B5" s="28">
-        <v>0.875</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>102</v>
@@ -4961,7 +5033,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E11" s="27">
         <v>9</v>
@@ -5065,7 +5137,7 @@
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D24" s="23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E24" s="27">
         <v>22</v>
@@ -5073,7 +5145,7 @@
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D25" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E25" s="27">
         <v>23</v>
@@ -5081,7 +5153,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D26" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E26" s="27">
         <v>24</v>
@@ -5089,7 +5161,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D27" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E27" s="27">
         <v>25</v>
@@ -5097,7 +5169,7 @@
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D28" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E28" s="27">
         <v>26</v>
@@ -5105,7 +5177,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D29" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E29" s="27">
         <v>27</v>
@@ -5113,7 +5185,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D30" s="23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E30" s="27">
         <v>28</v>
@@ -5121,7 +5193,7 @@
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D31" s="23" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E31" s="27">
         <v>29</v>
@@ -5129,7 +5201,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D32" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E32" s="27">
         <v>30</v>
@@ -5137,7 +5209,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E33" s="27">
         <v>31</v>
@@ -5154,9 +5226,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5176,7 +5248,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="7" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>48</v>
@@ -5255,12 +5327,18 @@
       <c r="G2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>273</v>
+      </c>
       <c r="J2" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="9"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -5360,7 +5438,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>205</v>
+        <v>298</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>199</v>
@@ -5759,7 +5837,7 @@
         <v>214</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -5935,7 +6013,7 @@
         <v>217</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -6171,7 +6249,7 @@
         <v>198</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -6308,7 +6386,7 @@
         <v>226</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -6438,10 +6516,9 @@
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="K36" s="9"/>
+      <c r="J36" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -6996,7 +7073,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7059,9 +7136,6 @@
       <c r="G2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -7079,9 +7153,6 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -7101,9 +7172,6 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="6" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -7123,9 +7191,6 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="6" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -7145,9 +7210,6 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="6" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -7167,9 +7229,6 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="6" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -7189,9 +7248,6 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="6" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -7212,7 +7268,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="6" t="s">
-        <v>258</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -7319,8 +7375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CFC106-4249-4BC9-9967-425037A65B0D}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7370,7 +7426,7 @@
         <v>130</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>88</v>
+        <v>280</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
@@ -7384,7 +7440,7 @@
         <v>134</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>88</v>
+        <v>281</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
@@ -7412,7 +7468,7 @@
         <v>118</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
@@ -7426,7 +7482,7 @@
         <v>119</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>88</v>
+        <v>278</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
@@ -7440,7 +7496,7 @@
         <v>117</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>88</v>
+        <v>282</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
@@ -7454,7 +7510,7 @@
         <v>120</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>88</v>
+        <v>277</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>1</v>
@@ -7468,7 +7524,7 @@
         <v>116</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>88</v>
+        <v>283</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>1</v>
@@ -7482,7 +7538,7 @@
         <v>144</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>88</v>
+        <v>279</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>1</v>
@@ -7496,7 +7552,7 @@
         <v>202</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>88</v>
+        <v>284</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>1</v>
@@ -7510,7 +7566,7 @@
         <v>135</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>88</v>
+        <v>285</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>1</v>
@@ -7524,7 +7580,7 @@
         <v>142</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>88</v>
+        <v>286</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>1</v>
@@ -7538,7 +7594,7 @@
         <v>146</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>88</v>
+        <v>287</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>1</v>
@@ -7552,7 +7608,7 @@
         <v>151</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>88</v>
+        <v>276</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>1</v>
@@ -7566,7 +7622,7 @@
         <v>128</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>88</v>
+        <v>288</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
@@ -7580,7 +7636,7 @@
         <v>132</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>88</v>
+        <v>289</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
@@ -7594,7 +7650,7 @@
         <v>143</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>88</v>
+        <v>290</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>1</v>
@@ -7608,7 +7664,7 @@
         <v>147</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>88</v>
+        <v>291</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>1</v>
@@ -7622,7 +7678,7 @@
         <v>149</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>88</v>
+        <v>292</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>1</v>
@@ -7636,7 +7692,7 @@
         <v>152</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>88</v>
+        <v>275</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>1</v>
@@ -7650,7 +7706,7 @@
         <v>124</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>88</v>
+        <v>293</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>1</v>
@@ -7664,7 +7720,7 @@
         <v>127</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>88</v>
+        <v>294</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>1</v>
@@ -7678,7 +7734,7 @@
         <v>123</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>88</v>
+        <v>295</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
@@ -7692,7 +7748,7 @@
         <v>129</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>88</v>
+        <v>296</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>1</v>
@@ -7706,7 +7762,7 @@
         <v>133</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>1</v>
@@ -7720,7 +7776,7 @@
         <v>136</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>88</v>
+        <v>280</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
@@ -7734,7 +7790,7 @@
         <v>121</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>1</v>
@@ -7748,7 +7804,7 @@
         <v>125</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>1</v>
@@ -7762,7 +7818,7 @@
         <v>138</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I30" s="1" t="b">
         <v>1</v>
@@ -7776,7 +7832,7 @@
         <v>140</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>1</v>
@@ -7790,7 +7846,7 @@
         <v>131</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>1</v>
@@ -7804,7 +7860,7 @@
         <v>139</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>1</v>
@@ -7818,7 +7874,7 @@
         <v>141</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>1</v>
@@ -7832,7 +7888,7 @@
         <v>145</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>1</v>
@@ -7846,7 +7902,7 @@
         <v>150</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -7860,7 +7916,7 @@
         <v>153</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>1</v>
@@ -7874,7 +7930,7 @@
         <v>122</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>1</v>
@@ -7888,7 +7944,7 @@
         <v>126</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>1</v>
@@ -7902,7 +7958,7 @@
         <v>148</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>1</v>
@@ -7916,7 +7972,7 @@
         <v>233</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>1</v>
@@ -7930,7 +7986,7 @@
         <v>235</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>1</v>
@@ -7944,7 +8000,7 @@
         <v>237</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>1</v>
@@ -7958,7 +8014,7 @@
         <v>239</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>1</v>
@@ -7972,7 +8028,7 @@
         <v>241</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>1</v>
@@ -7986,7 +8042,7 @@
         <v>137</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>1</v>
@@ -8000,7 +8056,7 @@
         <v>244</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I47" s="1" t="b">
         <v>1</v>
@@ -8014,7 +8070,7 @@
         <v>246</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>1</v>
@@ -8028,7 +8084,7 @@
         <v>248</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>1</v>
@@ -8042,7 +8098,7 @@
         <v>250</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>1</v>
@@ -8056,7 +8112,7 @@
         <v>252</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>1</v>
@@ -8070,7 +8126,7 @@
         <v>254</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>1</v>
@@ -8084,7 +8140,7 @@
         <v>256</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>88</v>
+        <v>274</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>1</v>
@@ -8103,7 +8159,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8169,10 +8225,10 @@
         <v>44405</v>
       </c>
       <c r="F2" s="19">
-        <v>0.39583333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G2" s="19">
-        <v>0.4375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solution.py updates, Optimisation.py created
</commit_message>
<xml_diff>
--- a/Dataset/N2OR_New.xlsx
+++ b/Dataset/N2OR_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1B1DE5-AE72-4971-AD48-E1D69059FF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08A5882-9D1E-491E-BA79-0D127D39124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -3357,6 +3357,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3366,12 +3378,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3380,6 +3386,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3393,22 +3405,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3425,6 +3425,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3447,17 +3450,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3826,7 +3826,7 @@
       <c r="E10" s="52"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="60" t="s">
         <v>112</v>
       </c>
       <c r="B11" s="51"/>
@@ -3849,347 +3849,347 @@
       <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="57"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
     </row>
     <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="61"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="61"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="61"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="43"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="63"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="63"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
+      <c r="A39" s="62"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="39"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="43"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="37"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="45"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="32"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="36"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="36"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="32"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="38"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="43"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="41"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="45"/>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="61"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
       <c r="E53" s="48"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
       <c r="E54" s="48"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="60" t="s">
+      <c r="A55" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="60" t="s">
+      <c r="A56" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="61"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
@@ -4198,418 +4198,448 @@
       <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="32"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="44"/>
-      <c r="C60" s="44"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="45"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="45"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="41"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="45"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="41"/>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="39"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="43"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="39"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="37"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="39"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="40" t="s">
+      <c r="A66" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="41"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="45"/>
     </row>
     <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="60"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="46"/>
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="D68" s="46"/>
-      <c r="E68" s="47"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="31"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="39"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="37"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="39"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="44"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="45"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="41"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="44"/>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="45"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="41"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="45"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="41"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="44"/>
-      <c r="B74" s="44"/>
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
-      <c r="E74" s="45"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="41"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="45"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="41"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="45"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="41"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="44"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="45"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="41"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="44"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="45"/>
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="41"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="62"/>
-      <c r="B79" s="62"/>
-      <c r="C79" s="62"/>
-      <c r="D79" s="62"/>
-      <c r="E79" s="63"/>
+      <c r="A79" s="46"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="46"/>
+      <c r="E79" s="47"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="39"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="37"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="39"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="45"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="41"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="45"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="41"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="45"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="41"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="45"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="45"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="41"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="45"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="41"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="45"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="40"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="41"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="45"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="40"/>
+      <c r="E89" s="41"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="46"/>
-      <c r="B90" s="46"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
-      <c r="E90" s="47"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="31"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="35" t="s">
+      <c r="A91" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="39"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="36"/>
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="37"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="39"/>
     </row>
     <row r="93" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="44" t="s">
+      <c r="A93" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="45"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="41"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="45"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
+      <c r="E94" s="41"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="45"/>
+      <c r="A95" s="40"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="41"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
+      <c r="A96" s="40"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="41"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="44"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="45"/>
+      <c r="A97" s="40"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="41"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="44"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="45"/>
+      <c r="A98" s="40"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="40"/>
+      <c r="D98" s="40"/>
+      <c r="E98" s="41"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="45"/>
+      <c r="A99" s="40"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="41"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="45"/>
+      <c r="A100" s="40"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="40"/>
+      <c r="D100" s="40"/>
+      <c r="E100" s="41"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="46"/>
-      <c r="B101" s="46"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="46"/>
-      <c r="E101" s="47"/>
+      <c r="A101" s="30"/>
+      <c r="B101" s="30"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="30"/>
+      <c r="E101" s="31"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="35" t="s">
+      <c r="A102" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B102" s="36"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="37"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="37"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
+      <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="44" t="s">
+      <c r="A104" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B104" s="44"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="45"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="40"/>
+      <c r="D104" s="40"/>
+      <c r="E104" s="41"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="44"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="45"/>
+      <c r="A105" s="40"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="40"/>
+      <c r="E105" s="41"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="44"/>
-      <c r="B106" s="44"/>
-      <c r="C106" s="44"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="45"/>
+      <c r="A106" s="40"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="40"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="41"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="44"/>
-      <c r="B107" s="44"/>
-      <c r="C107" s="44"/>
-      <c r="D107" s="44"/>
-      <c r="E107" s="45"/>
+      <c r="A107" s="40"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="40"/>
+      <c r="D107" s="40"/>
+      <c r="E107" s="41"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="44"/>
-      <c r="B108" s="44"/>
-      <c r="C108" s="44"/>
-      <c r="D108" s="44"/>
-      <c r="E108" s="45"/>
+      <c r="A108" s="40"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="40"/>
+      <c r="D108" s="40"/>
+      <c r="E108" s="41"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="44"/>
-      <c r="B109" s="44"/>
-      <c r="C109" s="44"/>
-      <c r="D109" s="44"/>
-      <c r="E109" s="45"/>
+      <c r="A109" s="40"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
+      <c r="E109" s="41"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="44"/>
-      <c r="B110" s="44"/>
-      <c r="C110" s="44"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="45"/>
+      <c r="A110" s="40"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="40"/>
+      <c r="D110" s="40"/>
+      <c r="E110" s="41"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="44"/>
-      <c r="B111" s="44"/>
-      <c r="C111" s="44"/>
-      <c r="D111" s="44"/>
-      <c r="E111" s="45"/>
+      <c r="A111" s="40"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="40"/>
+      <c r="D111" s="40"/>
+      <c r="E111" s="41"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="46"/>
-      <c r="B112" s="46"/>
-      <c r="C112" s="46"/>
-      <c r="D112" s="46"/>
-      <c r="E112" s="47"/>
+      <c r="A112" s="30"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="A46:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E39"/>
+    <mergeCell ref="A80:E81"/>
+    <mergeCell ref="A82:E89"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A53:E54"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A4:E10"/>
+    <mergeCell ref="A15:E16"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="A24:E26"/>
+    <mergeCell ref="A11:E13"/>
+    <mergeCell ref="A20:E21"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A27:E29"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A79:E79"/>
     <mergeCell ref="A112:E112"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A58:E59"/>
@@ -4626,36 +4656,6 @@
     <mergeCell ref="A71:E78"/>
     <mergeCell ref="A102:E103"/>
     <mergeCell ref="A104:E111"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A80:E81"/>
-    <mergeCell ref="A82:E89"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A53:E54"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A4:E10"/>
-    <mergeCell ref="A15:E16"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A17:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A22:E23"/>
-    <mergeCell ref="A24:E26"/>
-    <mergeCell ref="A11:E13"/>
-    <mergeCell ref="A20:E21"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A27:E29"/>
-    <mergeCell ref="A44:E45"/>
-    <mergeCell ref="A46:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4903,8 +4903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B4773B-09CB-4AE1-B7A2-EA1A4F4D3191}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4945,7 +4945,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4971,7 +4971,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -4985,7 +4985,7 @@
         <v>102</v>
       </c>
       <c r="E5" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4993,7 +4993,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="27">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -5001,7 +5001,7 @@
         <v>104</v>
       </c>
       <c r="E7" s="27">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -5009,7 +5009,7 @@
         <v>105</v>
       </c>
       <c r="E8" s="27">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -5017,7 +5017,7 @@
         <v>183</v>
       </c>
       <c r="E9" s="27">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -5025,7 +5025,7 @@
         <v>184</v>
       </c>
       <c r="E10" s="27">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -5033,7 +5033,7 @@
         <v>270</v>
       </c>
       <c r="E11" s="27">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -5041,7 +5041,7 @@
         <v>182</v>
       </c>
       <c r="E12" s="27">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -5049,7 +5049,7 @@
         <v>181</v>
       </c>
       <c r="E13" s="27">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -5057,7 +5057,7 @@
         <v>106</v>
       </c>
       <c r="E14" s="27">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -5065,7 +5065,7 @@
         <v>107</v>
       </c>
       <c r="E15" s="27">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -5073,7 +5073,7 @@
         <v>108</v>
       </c>
       <c r="E16" s="27">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.3">
@@ -5081,7 +5081,7 @@
         <v>109</v>
       </c>
       <c r="E17" s="27">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.3">
@@ -5089,7 +5089,7 @@
         <v>172</v>
       </c>
       <c r="E18" s="27">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.3">
@@ -5097,7 +5097,7 @@
         <v>110</v>
       </c>
       <c r="E19" s="27">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
@@ -5105,7 +5105,7 @@
         <v>180</v>
       </c>
       <c r="E20" s="27">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.3">
@@ -5113,7 +5113,7 @@
         <v>187</v>
       </c>
       <c r="E21" s="27">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.3">
@@ -5121,7 +5121,7 @@
         <v>188</v>
       </c>
       <c r="E22" s="27">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.3">
@@ -5129,7 +5129,7 @@
         <v>189</v>
       </c>
       <c r="E23" s="27">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.3">
@@ -5137,7 +5137,7 @@
         <v>261</v>
       </c>
       <c r="E24" s="27">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.3">
@@ -5145,7 +5145,7 @@
         <v>262</v>
       </c>
       <c r="E25" s="27">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.3">
@@ -5153,7 +5153,7 @@
         <v>259</v>
       </c>
       <c r="E26" s="27">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.3">
@@ -5161,7 +5161,7 @@
         <v>260</v>
       </c>
       <c r="E27" s="27">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.3">
@@ -5169,7 +5169,7 @@
         <v>263</v>
       </c>
       <c r="E28" s="27">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.3">
@@ -5177,7 +5177,7 @@
         <v>264</v>
       </c>
       <c r="E29" s="27">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.3">
@@ -5185,7 +5185,7 @@
         <v>265</v>
       </c>
       <c r="E30" s="27">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.3">
@@ -5193,7 +5193,7 @@
         <v>266</v>
       </c>
       <c r="E31" s="27">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.3">
@@ -5201,7 +5201,7 @@
         <v>267</v>
       </c>
       <c r="E32" s="27">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
@@ -5209,7 +5209,7 @@
         <v>268</v>
       </c>
       <c r="E33" s="27">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5224,8 +5224,8 @@
   <dimension ref="A1:T157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7063,7 +7063,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8319,7 +8319,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -8439,7 +8439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>